<commit_message>
fixed dates on mitigation2 pdf
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM2/risks/week7/fondo.xlsx
+++ b/PM2/risks/week7/fondo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM2\risks\week7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697C407D-74E9-4F98-8612-CC5F3F97F855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBCF779-A7E8-448A-900E-B17B336F0AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8AF350A-7B5E-4D18-9359-020966EFA052}"/>
   </bookViews>
@@ -419,42 +419,6 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -489,10 +453,46 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="44" fontId="1" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -710,7 +710,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>regression</c:v>
+            <c:v>Y = 3.6909 + 0.2242x</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1582,16 +1582,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1918,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157243EF-8961-4BF1-8A76-CD2EEF4EC089}">
   <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,62 +1928,62 @@
     <col min="3" max="3" width="7.5703125" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="2:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1992,197 +1992,197 @@
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="9">
         <f>(6/365)</f>
         <v>1.643835616438356E-2</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="16">
         <f>K4</f>
         <v>1800</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="21">
         <v>2</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="21">
         <v>6</v>
       </c>
-      <c r="I4" s="33">
+      <c r="I4" s="21">
         <v>1</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="21">
         <v>150</v>
       </c>
-      <c r="K4" s="34">
+      <c r="K4" s="22">
         <f>G4*H4*I4*J4</f>
         <v>1800</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="10">
         <v>0.63</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="16">
         <f t="shared" ref="F5:F20" si="0">K5</f>
         <v>57487.5</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="21">
         <v>2</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="21">
         <f>365*E5</f>
         <v>229.95</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="21">
         <v>1</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="21">
         <v>125</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5" s="22">
         <f>G5*H5*I5*J5</f>
         <v>57487.5</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="10">
         <f>2/365</f>
         <v>5.4794520547945206E-3</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="16">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="21">
         <v>8</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="21">
         <v>2</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="21">
         <v>1</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="21">
         <v>150</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="22">
         <f t="shared" ref="K6:K9" si="1">G6*H6*I6*J6</f>
         <v>2400</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="10">
         <v>0.1</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="16">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="21">
         <v>4</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="21">
         <v>1</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="21">
         <v>1</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="21">
         <v>150</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7" s="22">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="10">
         <v>0.7</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="16">
         <f t="shared" si="0"/>
         <v>76649.999999999985</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="21">
         <v>1</v>
       </c>
-      <c r="H8" s="33">
-        <f>365*E8</f>
+      <c r="H8" s="21">
+        <f t="shared" ref="H8:H19" si="2">365*E8</f>
         <v>255.49999999999997</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="21">
         <v>2</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="21">
         <v>150</v>
       </c>
-      <c r="K8" s="34">
+      <c r="K8" s="22">
         <f t="shared" si="1"/>
         <v>76649.999999999985</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="11"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="10">
         <v>0.8</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="16">
         <f t="shared" si="0"/>
         <v>175200</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="21">
         <v>2</v>
       </c>
-      <c r="H9" s="33">
-        <f>365*E9</f>
+      <c r="H9" s="21">
+        <f t="shared" si="2"/>
         <v>292</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="21">
         <v>1</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="21">
         <v>300</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9" s="22">
         <f t="shared" si="1"/>
         <v>175200</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="26" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -2191,33 +2191,33 @@
       <c r="D10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="11">
         <v>0.7</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="16">
         <f t="shared" si="0"/>
         <v>102199.99999999999</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="21">
         <v>2</v>
       </c>
-      <c r="H10" s="33">
-        <f>365*E10</f>
+      <c r="H10" s="21">
+        <f t="shared" si="2"/>
         <v>255.49999999999997</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="21">
         <v>2</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="21">
         <v>100</v>
       </c>
-      <c r="K10" s="34">
-        <f t="shared" ref="K10:K19" si="2">G10*H10*I10*J10</f>
+      <c r="K10" s="22">
+        <f t="shared" ref="K10:K19" si="3">G10*H10*I10*J10</f>
         <v>102199.99999999999</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="13"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
@@ -2227,96 +2227,96 @@
       <c r="E11" s="6">
         <v>3.2099999999999997E-2</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="16">
         <f t="shared" si="0"/>
         <v>878.73749999999984</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="21">
         <v>0.5</v>
       </c>
-      <c r="H11" s="33">
-        <f>365*E11</f>
+      <c r="H11" s="21">
+        <f t="shared" si="2"/>
         <v>11.716499999999998</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="21">
         <v>1</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="21">
         <v>150</v>
       </c>
-      <c r="K11" s="34">
-        <f t="shared" si="2"/>
+      <c r="K11" s="22">
+        <f t="shared" si="3"/>
         <v>878.73749999999984</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="11">
         <v>0.1</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="16">
         <f t="shared" si="0"/>
         <v>1825</v>
       </c>
-      <c r="G12" s="33">
+      <c r="G12" s="21">
         <v>0.5</v>
       </c>
-      <c r="H12" s="33">
-        <f>365*E12</f>
+      <c r="H12" s="21">
+        <f t="shared" si="2"/>
         <v>36.5</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="21">
         <v>1</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="21">
         <v>100</v>
       </c>
-      <c r="K12" s="34">
-        <f t="shared" si="2"/>
+      <c r="K12" s="22">
+        <f t="shared" si="3"/>
         <v>1825</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="11">
         <v>0.1</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="16">
         <f t="shared" si="0"/>
         <v>43800</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="21">
         <v>8</v>
       </c>
-      <c r="H13" s="33">
-        <f>365*E13</f>
+      <c r="H13" s="21">
+        <f t="shared" si="2"/>
         <v>36.5</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="21">
         <v>1</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="21">
         <v>150</v>
       </c>
-      <c r="K13" s="34">
-        <f t="shared" si="2"/>
+      <c r="K13" s="22">
+        <f t="shared" si="3"/>
         <v>43800</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="29" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -2325,99 +2325,99 @@
       <c r="D14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="12">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="16">
         <f t="shared" si="0"/>
         <v>2555</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="21">
         <v>1</v>
       </c>
-      <c r="H14" s="33">
-        <f>365*E14</f>
+      <c r="H14" s="21">
+        <f t="shared" si="2"/>
         <v>25.55</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="21">
         <v>1</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="21">
         <v>100</v>
       </c>
-      <c r="K14" s="34">
-        <f t="shared" si="2"/>
+      <c r="K14" s="22">
+        <f t="shared" si="3"/>
         <v>2555</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="12">
         <v>0.65</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="16">
         <f t="shared" si="0"/>
         <v>71175</v>
       </c>
-      <c r="G15" s="33">
+      <c r="G15" s="21">
         <v>2</v>
       </c>
-      <c r="H15" s="33">
-        <f>365*E15</f>
+      <c r="H15" s="21">
+        <f t="shared" si="2"/>
         <v>237.25</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="21">
         <v>1</v>
       </c>
-      <c r="J15" s="33">
+      <c r="J15" s="21">
         <v>150</v>
       </c>
-      <c r="K15" s="34">
-        <f t="shared" si="2"/>
+      <c r="K15" s="22">
+        <f t="shared" si="3"/>
         <v>71175</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="13">
         <v>0.4</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="16">
         <f t="shared" si="0"/>
         <v>14600</v>
       </c>
-      <c r="G16" s="33">
+      <c r="G16" s="21">
         <v>1</v>
       </c>
-      <c r="H16" s="33">
-        <f>365*E16</f>
+      <c r="H16" s="21">
+        <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="21">
         <v>1</v>
       </c>
-      <c r="J16" s="33">
+      <c r="J16" s="21">
         <v>100</v>
       </c>
-      <c r="K16" s="34">
-        <f t="shared" si="2"/>
+      <c r="K16" s="22">
+        <f t="shared" si="3"/>
         <v>14600</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="32" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -2426,110 +2426,110 @@
       <c r="D17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="14">
         <f>(2/365)</f>
         <v>5.4794520547945206E-3</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="16">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G17" s="21">
         <v>1</v>
       </c>
-      <c r="H17" s="33">
-        <f>365*E17</f>
+      <c r="H17" s="21">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="21">
         <v>1</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="21">
         <v>150</v>
       </c>
-      <c r="K17" s="34">
-        <f t="shared" si="2"/>
+      <c r="K17" s="22">
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="19"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="14">
         <v>0.09</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="16">
         <f t="shared" si="0"/>
         <v>19710</v>
       </c>
-      <c r="G18" s="33">
+      <c r="G18" s="21">
         <v>2</v>
       </c>
-      <c r="H18" s="33">
-        <f>365*E18</f>
+      <c r="H18" s="21">
+        <f t="shared" si="2"/>
         <v>32.85</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="21">
         <v>1</v>
       </c>
-      <c r="J18" s="33">
+      <c r="J18" s="21">
         <v>300</v>
       </c>
-      <c r="K18" s="34">
-        <f t="shared" si="2"/>
+      <c r="K18" s="22">
+        <f t="shared" si="3"/>
         <v>19710</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="14">
         <v>0.12</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="16">
         <f t="shared" si="0"/>
         <v>1095</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="21">
         <v>0.25</v>
       </c>
-      <c r="H19" s="33">
-        <f>365*E19</f>
+      <c r="H19" s="21">
+        <f t="shared" si="2"/>
         <v>43.8</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="21">
         <v>1</v>
       </c>
-      <c r="J19" s="33">
+      <c r="J19" s="21">
         <v>100</v>
       </c>
-      <c r="K19" s="34">
-        <f t="shared" si="2"/>
+      <c r="K19" s="22">
+        <f t="shared" si="3"/>
         <v>1095</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="18">
         <f t="shared" si="0"/>
         <v>572276.23750000005</v>
       </c>
       <c r="J20" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="27">
+      <c r="K20" s="15">
         <f>SUM(K4:K19)</f>
         <v>572276.23750000005</v>
       </c>
@@ -2551,8 +2551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FAD972-686B-48C9-9D06-FB3011F4B66E}">
   <dimension ref="B1:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update: risk final v1
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM2/risks/week7/fondo.xlsx
+++ b/PM2/risks/week7/fondo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM2\risks\week7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBCF779-A7E8-448A-900E-B17B336F0AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82D50E9-14A8-40EA-8DD8-F5C498D07E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8AF350A-7B5E-4D18-9359-020966EFA052}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E8AF350A-7B5E-4D18-9359-020966EFA052}"/>
   </bookViews>
   <sheets>
     <sheet name="EMVs" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +237,14 @@
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -388,14 +396,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -495,12 +504,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1918,7 +1929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157243EF-8961-4BF1-8A76-CD2EEF4EC089}">
   <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -2551,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FAD972-686B-48C9-9D06-FB3011F4B66E}">
   <dimension ref="B1:J42"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2678,7 +2689,7 @@
         <f t="shared" si="0"/>
         <v>4.1393000000000004</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="37" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2780,8 +2791,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J33" r:id="rId1" xr:uid="{45622CD8-F19A-4AC6-8C95-7BBB3233B232}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>